<commit_message>
page modification droits fonctionelle
</commit_message>
<xml_diff>
--- a/heure de travaille mathieu.xlsx
+++ b/heure de travaille mathieu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenon\Desktop\Siteradio\partieconnexionInscription\Uwamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu Zenone\Desktop\Siteradio\partieconnexionInscription\Uwamp\www\ProjetRadioGit\ProjetRadioPhp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE920F4A-6D23-4CE4-8043-A6D7A251A09A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BFCB4E-FCBE-4A24-A359-13262E600292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>5h bd 25/02</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>page modifier droits commencé</t>
+  </si>
+  <si>
+    <t>page modifier droits finis</t>
   </si>
 </sst>
 </file>
@@ -444,40 +447,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -485,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -500,10 +503,10 @@
       </c>
       <c r="F6">
         <f>SUM(B7:B32)</f>
-        <v>98.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43845</v>
       </c>
@@ -514,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43855</v>
       </c>
@@ -525,7 +528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43857</v>
       </c>
@@ -536,7 +539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43869</v>
       </c>
@@ -547,7 +550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43870</v>
       </c>
@@ -558,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43871</v>
       </c>
@@ -569,7 +572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43873</v>
       </c>
@@ -580,7 +583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43876</v>
       </c>
@@ -591,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43878</v>
       </c>
@@ -602,7 +605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -613,7 +616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43886</v>
       </c>
@@ -624,7 +627,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43887</v>
       </c>
@@ -635,7 +638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43888</v>
       </c>
@@ -646,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43891</v>
       </c>
@@ -657,7 +660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -668,7 +671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43893</v>
       </c>
@@ -679,7 +682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43897</v>
       </c>
@@ -690,7 +693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43898</v>
       </c>
@@ -701,7 +704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43899</v>
       </c>
@@ -712,7 +715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43899</v>
       </c>
@@ -723,7 +726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43900</v>
       </c>
@@ -734,7 +737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43907</v>
       </c>
@@ -745,7 +748,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43908</v>
       </c>
@@ -756,7 +759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43909</v>
       </c>
@@ -767,7 +770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43912</v>
       </c>
@@ -776,6 +779,17 @@
       </c>
       <c r="C31" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Premiere version du site complétement fonctionelle
</commit_message>
<xml_diff>
--- a/heure de travaille mathieu.xlsx
+++ b/heure de travaille mathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu Zenone\Desktop\Siteradio\partieconnexionInscription\Uwamp\www\ProjetRadioGit\ProjetRadioPhp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14B186B-5C7F-401F-8EFC-A88BFD6A6AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC6E2A-0A4C-4094-95A3-A637017E2056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>5h bd 25/02</t>
   </si>
@@ -98,12 +98,6 @@
     <t>etude Jquerry</t>
   </si>
   <si>
-    <t>etude DropFile</t>
-  </si>
-  <si>
-    <t>outil DropFile maitrisé et modilation de model pour future implémentation</t>
-  </si>
-  <si>
     <t>integration de différente partie refonte de l'organistation du site</t>
   </si>
   <si>
@@ -141,6 +135,21 @@
   </si>
   <si>
     <t>Archivage desarchivage, navigabilité visuelle et bug fix</t>
+  </si>
+  <si>
+    <t>abandon de la library dropzone page ajout theme/emission podcast fonctionelle</t>
+  </si>
+  <si>
+    <t>page modifier en cours de construction modifier theme et emission fonctionelle</t>
+  </si>
+  <si>
+    <t>etude Dropzone</t>
+  </si>
+  <si>
+    <t>outil Dropzone maitrisé et modilation de model pour future implémentation</t>
+  </si>
+  <si>
+    <t>page modifier fonctionelle site fonctionelle v1</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,11 +520,11 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <f>SUM(B7:B39)</f>
-        <v>118.5</v>
+        <v>140.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,7 +722,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +755,7 @@
         <v>2.5</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +854,40 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>